<commit_message>
adicionando odds como classificador
</commit_message>
<xml_diff>
--- a/base de dados e códigos/comparacao_algoritmos_machine_learning.xlsx
+++ b/base de dados e códigos/comparacao_algoritmos_machine_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André\Documents\Eng. Computação\2020.1\TCC\base de dados e códigos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD292B3-5A85-413A-91D6-DF1B0D35339B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1D9E06-3C94-43D1-9C8C-A01C561153E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>Árvore</t>
   </si>
   <si>
-    <t>Regras</t>
-  </si>
-  <si>
     <t>kNN</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Odds</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,22 +705,22 @@
         <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="2" t="s">
@@ -730,22 +730,22 @@
         <v>36</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="R5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -761,7 +761,9 @@
       <c r="D6" s="4">
         <v>0.64265859184384799</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4">
+        <v>0.55419135587312596</v>
+      </c>
       <c r="F6" s="4">
         <v>0.56335395608225802</v>
       </c>
@@ -778,15 +780,15 @@
       </c>
       <c r="L6" s="6">
         <f t="shared" ref="L6:L35" si="1">_xlfn.RANK.AVG(C6,B6:I6)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M6" s="6">
         <f>_xlfn.RANK.AVG(D6,B6:I6)</f>
         <v>1</v>
       </c>
-      <c r="N6" s="6" t="e">
+      <c r="N6" s="6">
         <f t="shared" ref="N6:N35" si="2">_xlfn.RANK.AVG(E6,B6:I6)</f>
-        <v>#N/A</v>
+        <v>6</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" ref="O6:O35" si="3">_xlfn.RANK.AVG(F6,B6:I6)</f>
@@ -818,7 +820,9 @@
       <c r="D7" s="4">
         <v>0.62163210177762196</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F7" s="4">
         <v>0.55024834437086001</v>
       </c>
@@ -831,23 +835,23 @@
       </c>
       <c r="K7" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" ref="M7:M35" si="7">_xlfn.RANK.AVG(D7,B7:I7)</f>
         <v>1</v>
       </c>
-      <c r="N7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N7" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P7" s="6" t="e">
         <f t="shared" si="4"/>
@@ -875,7 +879,9 @@
       <c r="D8" s="4">
         <v>0.632811955385151</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>0.55404757755315404</v>
+      </c>
       <c r="F8" s="4">
         <v>0.56412077378877601</v>
       </c>
@@ -888,19 +894,19 @@
       </c>
       <c r="K8" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N8" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="3"/>
@@ -932,7 +938,9 @@
       <c r="D9" s="4">
         <v>0.63543046357615895</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4">
+        <v>0.55420442662948699</v>
+      </c>
       <c r="F9" s="4">
         <v>0.55159463227605399</v>
       </c>
@@ -945,23 +953,23 @@
       </c>
       <c r="K9" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N9" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9" s="6" t="e">
         <f t="shared" si="4"/>
@@ -989,7 +997,9 @@
       <c r="D10" s="4">
         <v>0.63211484837922605</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>0.55421314046706105</v>
+      </c>
       <c r="F10" s="4">
         <v>0.56210352039037903</v>
       </c>
@@ -1002,19 +1012,19 @@
       </c>
       <c r="K10" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M10" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N10" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="3"/>
@@ -1046,7 +1056,9 @@
       <c r="D11" s="4">
         <v>0.642601951899616</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>0.55420878354827396</v>
+      </c>
       <c r="F11" s="4">
         <v>0.55743290345067897</v>
       </c>
@@ -1069,9 +1081,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N11" s="6">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="3"/>
@@ -1103,7 +1115,9 @@
       <c r="D12" s="4">
         <v>0.64137765772045996</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>0.55418264203555201</v>
+      </c>
       <c r="F12" s="4">
         <v>0.56473074241896104</v>
       </c>
@@ -1116,19 +1130,19 @@
       </c>
       <c r="K12" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N12" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="3"/>
@@ -1160,7 +1174,9 @@
       <c r="D13" s="4">
         <v>0.62740066225165503</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4">
+        <v>0.55407371906587599</v>
+      </c>
       <c r="F13" s="4">
         <v>0.54688044614848297</v>
       </c>
@@ -1173,23 +1189,23 @@
       </c>
       <c r="K13" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N13" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P13" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1217,7 +1233,9 @@
       <c r="D14" s="4">
         <v>0.63342628093412301</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4">
+        <v>0.55416957127919098</v>
+      </c>
       <c r="F14" s="4">
         <v>0.56605088881143195</v>
       </c>
@@ -1234,15 +1252,15 @@
       </c>
       <c r="L14" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="3"/>
@@ -1274,7 +1292,9 @@
       <c r="D15" s="4">
         <v>0.62879051934471897</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>0.554165214360404</v>
+      </c>
       <c r="F15" s="4">
         <v>0.56539735099337696</v>
       </c>
@@ -1291,15 +1311,15 @@
       </c>
       <c r="L15" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N15" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="3"/>
@@ -1331,7 +1351,9 @@
       <c r="D16" s="4">
         <v>0.63673318229348197</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>0.55414342976646902</v>
+      </c>
       <c r="F16" s="4">
         <v>0.55217845939351695</v>
       </c>
@@ -1344,7 +1366,7 @@
       </c>
       <c r="K16" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="1"/>
@@ -1354,13 +1376,13 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N16" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P16" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1388,7 +1410,9 @@
       <c r="D17" s="4">
         <v>0.634733356570233</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F17" s="4">
         <v>0.56009933774834397</v>
       </c>
@@ -1405,15 +1429,15 @@
       </c>
       <c r="L17" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N17" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" si="3"/>
@@ -1445,7 +1469,9 @@
       <c r="D18" s="4">
         <v>0.63210613454165199</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>0.55418264203555201</v>
+      </c>
       <c r="F18" s="4">
         <v>0.552152317880794</v>
       </c>
@@ -1462,19 +1488,19 @@
       </c>
       <c r="L18" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N18" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P18" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1502,7 +1528,9 @@
       <c r="D19" s="4">
         <v>0.62947019867549603</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>0.55415650052283005</v>
+      </c>
       <c r="F19" s="4">
         <v>0.56546270477518201</v>
       </c>
@@ -1515,19 +1543,19 @@
       </c>
       <c r="K19" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N19" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O19" s="6">
         <f t="shared" si="3"/>
@@ -1559,7 +1587,9 @@
       <c r="D20" s="4">
         <v>0.62743116068316396</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4">
+        <v>0.55416085744161703</v>
+      </c>
       <c r="F20" s="4">
         <v>0.56272220285813801</v>
       </c>
@@ -1572,19 +1602,19 @@
       </c>
       <c r="K20" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L20" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M20" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N20" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O20" s="6">
         <f t="shared" si="3"/>
@@ -1616,7 +1646,9 @@
       <c r="D21" s="4">
         <v>0.62148832345765004</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4">
+        <v>0.55419135587312596</v>
+      </c>
       <c r="F21" s="4">
         <v>0.55411293133495998</v>
       </c>
@@ -1629,23 +1661,23 @@
       </c>
       <c r="K21" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M21" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N21" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N21" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O21" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P21" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1673,7 +1705,9 @@
       <c r="D22" s="4">
         <v>0.62620250958522095</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4">
+        <v>0.554221854304635</v>
+      </c>
       <c r="F22" s="4">
         <v>0.56603346113628406</v>
       </c>
@@ -1686,19 +1720,19 @@
       </c>
       <c r="K22" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M22" s="6">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N22" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N22" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O22" s="6">
         <f t="shared" si="3"/>
@@ -1730,7 +1764,9 @@
       <c r="D23" s="4">
         <v>0.63797490414778601</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F23" s="4">
         <v>0.55413471592889496</v>
       </c>
@@ -1743,23 +1779,23 @@
       </c>
       <c r="K23" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L23" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M23" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N23" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N23" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O23" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P23" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1787,7 +1823,9 @@
       <c r="D24" s="4">
         <v>0.62815440920181198</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F24" s="4">
         <v>0.55420878354827396</v>
       </c>
@@ -1800,19 +1838,19 @@
       </c>
       <c r="K24" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M24" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N24" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N24" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O24" s="6">
         <f t="shared" si="3"/>
@@ -1844,7 +1882,9 @@
       <c r="D25" s="4">
         <v>0.62815440920181198</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F25" s="4">
         <v>0.56532764029278404</v>
       </c>
@@ -1857,19 +1897,19 @@
       </c>
       <c r="K25" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M25" s="6">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N25" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N25" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="3"/>
@@ -1901,7 +1941,9 @@
       <c r="D26" s="4">
         <v>0.63733008016730497</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4">
+        <v>0.55411293133495998</v>
+      </c>
       <c r="F26" s="4">
         <v>0.56078773091669498</v>
       </c>
@@ -1914,19 +1956,19 @@
       </c>
       <c r="K26" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N26" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N26" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="3"/>
@@ -1958,7 +2000,9 @@
       <c r="D27" s="4">
         <v>0.63016294876263501</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F27" s="4">
         <v>0.56403799233182295</v>
       </c>
@@ -1971,7 +2015,7 @@
       </c>
       <c r="K27" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="1"/>
@@ -1981,9 +2025,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N27" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N27" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O27" s="6">
         <f t="shared" si="3"/>
@@ -2015,7 +2059,9 @@
       <c r="D28" s="4">
         <v>0.63279017079121602</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4">
+        <v>0.55416085744161703</v>
+      </c>
       <c r="F28" s="4">
         <v>0.55089752527012803</v>
       </c>
@@ -2032,19 +2078,19 @@
       </c>
       <c r="L28" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M28" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N28" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N28" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O28" s="6">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P28" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2072,7 +2118,9 @@
       <c r="D29" s="4">
         <v>0.63338271174625205</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>0.55407807598466297</v>
+      </c>
       <c r="F29" s="4">
         <v>0.56010369466713095</v>
       </c>
@@ -2089,15 +2137,15 @@
       </c>
       <c r="L29" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M29" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N29" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N29" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O29" s="6">
         <f t="shared" si="3"/>
@@ -2129,7 +2177,9 @@
       <c r="D30" s="4">
         <v>0.64271523178807899</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F30" s="4">
         <v>0.56605088881143195</v>
       </c>
@@ -2152,9 +2202,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N30" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N30" s="6">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="3"/>
@@ -2186,7 +2236,9 @@
       <c r="D31" s="4">
         <v>0.62874259323806203</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4">
+        <v>0.55410857441617201</v>
+      </c>
       <c r="F31" s="4">
         <v>0.55747211571976296</v>
       </c>
@@ -2199,19 +2251,19 @@
       </c>
       <c r="K31" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M31" s="6">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N31" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N31" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O31" s="6">
         <f t="shared" si="3"/>
@@ -2243,7 +2295,9 @@
       <c r="D32" s="4">
         <v>0.64074154757755297</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4">
+        <v>0.55413907284768205</v>
+      </c>
       <c r="F32" s="4">
         <v>0.55343325200418203</v>
       </c>
@@ -2256,23 +2310,23 @@
       </c>
       <c r="K32" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M32" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N32" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N32" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O32" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P32" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2300,7 +2354,9 @@
       <c r="D33" s="4">
         <v>0.634079818752178</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4">
+        <v>0.55414778668525599</v>
+      </c>
       <c r="F33" s="4">
         <v>0.554165214360404</v>
       </c>
@@ -2313,19 +2369,19 @@
       </c>
       <c r="K33" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M33" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N33" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N33" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O33" s="6">
         <f t="shared" si="3"/>
@@ -2357,7 +2413,9 @@
       <c r="D34" s="4">
         <v>0.62687783199721103</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F34" s="4">
         <v>0.55153363541303502</v>
       </c>
@@ -2374,19 +2432,19 @@
       </c>
       <c r="L34" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M34" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N34" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N34" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O34" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P34" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2414,7 +2472,9 @@
       <c r="D35" s="4">
         <v>0.63078598814917997</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>0.55414342976646902</v>
+      </c>
       <c r="F35" s="4">
         <v>0.56077466016033395</v>
       </c>
@@ -2427,19 +2487,19 @@
       </c>
       <c r="K35" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M35" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N35" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N35" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O35" s="6">
         <f t="shared" si="3"/>
@@ -2474,9 +2534,9 @@
         <f t="shared" si="8"/>
         <v>0.63261008481468517</v>
       </c>
-      <c r="E36" s="8" t="e">
+      <c r="E36" s="8">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0.55415867898222337</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="8"/>
@@ -2496,23 +2556,23 @@
       </c>
       <c r="K36" s="9">
         <f t="shared" ref="K36:R36" si="9">AVERAGE(K6:K35)</f>
-        <v>5</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="L36" s="9">
         <f t="shared" si="9"/>
-        <v>5.6</v>
+        <v>6.4666666666666668</v>
       </c>
       <c r="M36" s="9">
         <f t="shared" si="9"/>
         <v>1.1333333333333333</v>
       </c>
-      <c r="N36" s="9" t="e">
+      <c r="N36" s="9">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>5.1333333333333337</v>
       </c>
       <c r="O36" s="9">
         <f t="shared" si="9"/>
-        <v>4.4000000000000004</v>
+        <v>4.7333333333333334</v>
       </c>
       <c r="P36" s="9" t="e">
         <f t="shared" si="9"/>
@@ -2536,22 +2596,22 @@
         <v>36</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="G37" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="H37" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>